<commit_message>
Update hw3.xlsx with pricing results
</commit_message>
<xml_diff>
--- a/xlsx/hw3.xlsx
+++ b/xlsx/hw3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\xlladdins\xll_ml\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27228\source\repos\xll_ml\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{368A1F7E-5C01-40F8-BDD5-9984332E47CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A28885-22FC-4FEF-87BA-6FA47AD98B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22276" windowHeight="13996" xr2:uid="{EA092A42-1670-4D44-86F1-B9E7694F8A62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EA092A42-1670-4D44-86F1-B9E7694F8A62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>f</t>
   </si>
@@ -82,6 +79,22 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>Strike</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moneyness</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Put</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -89,22 +102,29 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="&quot;0x&quot;#"/>
+    <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="63"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -127,7 +147,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -136,14 +156,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Handle" xfId="1" xr:uid="{1D654BEF-DD87-407E-A523-E3474ECC1167}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -227,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,52 +563,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE06CDEE-4F3C-473F-9F8B-5F0D6CBFE894}">
-  <dimension ref="B3:C7"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17.5"/>
   <cols>
-    <col min="1" max="1" width="3.578125" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" cm="1">
+        <f t="array" ref="E3:E11">_xlfn.SEQUENCE(9,1,80,5)</f>
+        <v>80</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3:F11">_xlfn.MAP(_xlfn.ANCHORARRAY(E3),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.MONEYNESS(f,s,_xlpm.k,m)))</f>
+        <v>-2.1814355131420968</v>
+      </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3:G11">_xlfn.MAP(_xlfn.ANCHORARRAY(E3),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.PUT(f,s,_xlpm.k,m)))</f>
+        <v>3.9913489502149124E-2</v>
+      </c>
+      <c r="H3" cm="1">
+        <f t="array" ref="H3:H11">_xlfn.MAP(_xlfn.ANCHORARRAY(E3),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.PUT(f,s,_xlpm.k,m)))</f>
+        <v>3.9913489502149124E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4">
+        <v>85</v>
+      </c>
+      <c r="F4">
+        <v>-1.5751892949777493</v>
+      </c>
+      <c r="G4">
+        <v>0.20169020324580078</v>
+      </c>
+      <c r="H4">
+        <v>0.20169020324580078</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>-1.0036051565782627</v>
+      </c>
+      <c r="G5">
+        <v>0.7123773837400833</v>
+      </c>
+      <c r="H5">
+        <v>0.7123773837400833</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" cm="1">
         <f t="array" ref="C6">_xll.\OPTION.NORMAL()</f>
-        <v>3016670213392</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+        <v>2313249358256</v>
+      </c>
+      <c r="E6">
+        <v>95</v>
+      </c>
+      <c r="F6">
+        <v>-0.46293294387550571</v>
+      </c>
+      <c r="G6">
+        <v>1.8880683097281832</v>
+      </c>
+      <c r="H6">
+        <v>1.8880683097281832</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -596,8 +682,77 @@
         <f t="array" ref="C7">_xll.OPTION.BLACK.PUT(f, s, k, m)</f>
         <v>3.9877746125013118</v>
       </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="G7">
+        <v>3.9877746125013118</v>
+      </c>
+      <c r="H7">
+        <v>3.9877746125013118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="E8">
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>0.53790164169432031</v>
+      </c>
+      <c r="G8">
+        <v>7.0640245213143373</v>
+      </c>
+      <c r="H8">
+        <v>7.0640245213143373</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>1.0031017980432493</v>
+      </c>
+      <c r="G9">
+        <v>10.953943365573252</v>
+      </c>
+      <c r="H9">
+        <v>10.953943365573252</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="E10">
+        <v>115</v>
+      </c>
+      <c r="F10">
+        <v>1.4476194237515863</v>
+      </c>
+      <c r="G10">
+        <v>15.394940132447118</v>
+      </c>
+      <c r="H10">
+        <v>15.394940132447118</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="E11">
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <v>1.8732155679395459</v>
+      </c>
+      <c r="G11">
+        <v>20.147335155685013</v>
+      </c>
+      <c r="H11">
+        <v>20.147335155685013</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>